<commit_message>
add features on Relasi
</commit_message>
<xml_diff>
--- a/uploads/import/format/guru.xlsx
+++ b/uploads/import/format/guru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cbt\uploads\import\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB5A4B-2B7B-4D52-83F0-B200B0C87188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC8BDC8-06A4-4A8B-A5A4-E6D00C9DEC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>nip</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>nama_guru</t>
-  </si>
-  <si>
-    <t>mapel_id</t>
   </si>
 </sst>
 </file>
@@ -406,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -417,12 +414,11 @@
     <col min="1" max="1" width="15.796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.69921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.69921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.19921875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="9" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -432,14 +428,11 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:3">
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:3">
       <c r="C3" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix master data & import (Guru, Siswa, Penempatan) * CRUD Distribusi Siswa
</commit_message>
<xml_diff>
--- a/uploads/import/format/guru.xlsx
+++ b/uploads/import/format/guru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cbt\uploads\import\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC8BDC8-06A4-4A8B-A5A4-E6D00C9DEC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51235AD-66EC-4CAD-8604-2D1680681E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,14 +406,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="15.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.69921875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>

</xml_diff>